<commit_message>
added result file download
</commit_message>
<xml_diff>
--- a/validator/result.xlsx
+++ b/validator/result.xlsx
@@ -861,10 +861,10 @@
         <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>238</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28">
@@ -893,10 +893,10 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1034</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="30">
@@ -941,10 +941,10 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33">
@@ -989,10 +989,10 @@
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>4417</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="36">
@@ -1053,10 +1053,10 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40">
@@ -1069,10 +1069,10 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41">
@@ -1101,10 +1101,10 @@
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>8233</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>8233</v>
       </c>
     </row>
     <row r="43">
@@ -1133,10 +1133,10 @@
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>1806</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="45">
@@ -1165,10 +1165,10 @@
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>2812</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>2812</v>
       </c>
     </row>
     <row r="47">
@@ -1245,10 +1245,10 @@
         <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>1956</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="52">
@@ -1293,10 +1293,10 @@
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55">
@@ -1453,10 +1453,10 @@
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65">
@@ -1565,10 +1565,10 @@
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>946</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>946</v>
       </c>
     </row>
     <row r="72">
@@ -1581,10 +1581,10 @@
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>7764</v>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>7764</v>
       </c>
     </row>
     <row r="73">
@@ -1613,10 +1613,10 @@
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75">
@@ -1693,10 +1693,10 @@
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80">
@@ -1773,10 +1773,10 @@
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>3143</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>3143</v>
       </c>
     </row>
     <row r="85">
@@ -1805,10 +1805,10 @@
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>1285</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="87">
@@ -1837,10 +1837,10 @@
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="89">
@@ -1965,10 +1965,10 @@
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="97">
@@ -2013,10 +2013,10 @@
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
+        <v>1085</v>
       </c>
       <c r="D99" t="n">
-        <v>0</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="100">
@@ -2045,10 +2045,10 @@
         <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="102">
@@ -2093,10 +2093,10 @@
         <v>0</v>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D104" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105">
@@ -2141,10 +2141,10 @@
         <v>0</v>
       </c>
       <c r="C107" t="n">
-        <v>0</v>
+        <v>4888</v>
       </c>
       <c r="D107" t="n">
-        <v>0</v>
+        <v>4888</v>
       </c>
     </row>
     <row r="108">
@@ -2205,10 +2205,10 @@
         <v>0</v>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>248415</v>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>248415</v>
       </c>
     </row>
     <row r="112">
@@ -2221,10 +2221,10 @@
         <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113">
@@ -2317,10 +2317,10 @@
         <v>0</v>
       </c>
       <c r="C118" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
     </row>
     <row r="119">

</xml_diff>